<commit_message>
PCA featureset and model fitting in main
</commit_message>
<xml_diff>
--- a/Analysis Results/ML project.xlsx
+++ b/Analysis Results/ML project.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">datsets\models</t>
   </si>
@@ -61,10 +61,19 @@
     <t xml:space="preserve">Original dataset</t>
   </si>
   <si>
+    <t xml:space="preserve">continuous vars only</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logarithms</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ratios and logartihms</t>
   </si>
   <si>
-    <t xml:space="preserve">Corelation analysis</t>
+    <t xml:space="preserve">uncorrelated vars</t>
   </si>
   <si>
     <t xml:space="preserve">PCA</t>
@@ -115,7 +124,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,7 +140,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF6AA84F"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
     <fill>
@@ -144,6 +153,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC33"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -181,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,6 +220,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,7 +245,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -260,7 +289,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF6AA84F"/>
       <rgbColor rgb="FF003300"/>
@@ -279,25 +308,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -358,17 +386,17 @@
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -402,6 +430,54 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>